<commit_message>
:memo: add more course material
</commit_message>
<xml_diff>
--- a/day15 内置和开发规范/代码和作业答案/课堂代码/db.xlsx
+++ b/day15 内置和开发规范/代码和作业答案/课堂代码/db.xlsx
@@ -2,33 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-31660" yWindow="1980" windowWidth="30720" windowHeight="18740" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -56,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -419,67 +413,77 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
-  <cols>
-    <col width="8" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="36.5" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="22" bestFit="1" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>root</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0dcda0307a535bc6903fb1c909676d3a</t>
+          <t>24034476e99d1aa26614c9e7902ae2700316c6709aeaedb24e79231968521b7d</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2021-01-04 17:24:04</t>
+          <t>2022-02-25 14:29:10</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>A4nf3I8M</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>wupeiq</t>
+          <t>Achuan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>00df0422145ac32d58c193902c23be30</t>
+          <t>91dfd8e0b70f8008238d780a57a64d17b5758031dd4b69ec9122644a3a45ea3c</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2021-01-04 17:24:08</t>
+          <t>2022-02-25 14:29:14</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>R9HrMT2z</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>alex</t>
+          <t>Achuan-2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>b94d015526e6d5ef60ffff35d5ad9017</t>
+          <t>d01ea24f3c2e92c641b8e142cd3636c694690d7d655b0c3295f358fc9ac81ffc</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2021-01-04 17:24:33</t>
+          <t>2022-02-25 14:31:18</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>v3GjYw81</t>
         </is>
       </c>
     </row>

</xml_diff>